<commit_message>
implement changes in the docx and code
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE\OneDrive\Desktop\Facultate\Semestrul 6\VVSS\infinity_inventory_vvss\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C66FA24-221E-457A-96FC-FC9B97EA6695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957F5768-AFBD-4BE0-884F-E069253B24FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -131,9 +131,6 @@
     <t>R07</t>
   </si>
   <si>
-    <t>No additional information is given about the file structure. The requirements should mention the size, the name, the contents and the number of items in the file</t>
-  </si>
-  <si>
     <t>R01</t>
   </si>
   <si>
@@ -213,19 +210,29 @@
   </si>
   <si>
     <t>BufferedReaders should be used with try-with-resources or it should be closed in a finally block</t>
+  </si>
+  <si>
+    <t>No additional information is given about the file structure. The requirements should mention the size, the name, and the contents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -404,79 +411,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +795,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +841,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
@@ -851,7 +859,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="17">
         <v>233</v>
@@ -862,14 +870,14 @@
         <v>9</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" s="17">
         <v>233</v>
@@ -904,7 +912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -915,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -924,13 +932,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -939,13 +947,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -958,7 +966,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1074,7 +1082,7 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1144,7 +1152,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
@@ -1162,7 +1170,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="17">
         <v>233</v>
@@ -1173,14 +1181,14 @@
         <v>10</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" s="17">
         <v>233</v>
@@ -1220,11 +1228,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1233,11 +1241,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1246,11 +1254,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1385,7 +1393,7 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1409,8 +1417,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1464,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
@@ -1474,7 +1482,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1485,14 +1493,14 @@
         <v>9</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1532,13 +1540,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1547,13 +1555,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1562,13 +1570,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1738,7 +1746,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="36" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
convert repo to singleton and fix bugs
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE\OneDrive\Desktop\Facultate\Semestrul 6\VVSS\infinity_inventory_vvss\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F084FE-2AC2-4F54-B9E4-01E30DD392F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECFA2D9-EF79-4ADA-8E86-97E80BF0FEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
-  </si>
-  <si>
     <t>R07</t>
   </si>
   <si>
@@ -173,15 +170,9 @@
     <t>A02</t>
   </si>
   <si>
-    <t>A09</t>
-  </si>
-  <si>
     <t>The validators should be in their own packages</t>
   </si>
   <si>
-    <t>Domain entities should be created by the services, not the repositories</t>
-  </si>
-  <si>
     <t>C06</t>
   </si>
   <si>
@@ -222,13 +213,105 @@
   </si>
   <si>
     <t>There is no exception handling specified. Solution: make a separate Exception class for each Domain class. Each class that uses a certain Domain class may throw the respective exception class (dependency annotated with &lt;&lt;throws&gt;&gt;&gt;.</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>InventoryRepository.java/line146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">				while(index&lt;list.size()-1){
+					line=line+list.get(index).getPartId()+":";
+					index++;
+				}</t>
+  </si>
+  <si>
+    <t>StringBuilder builder = new StringBuilder();
+				for (int i = 0; i &lt; list.size(); i++) {
+					builder.append(list.get(i).getPartId());
+					if (i &lt; list.size() - 1) {
+						builder.append(":");
+					}
+				}
+				if (index==list.size()-1) {
+					line+=builder.toString();
+				} else {
+					line+=builder.toString();
+				}</t>
+  </si>
+  <si>
+    <t>InventoryRepository.java/line23</t>
+  </si>
+  <si>
+    <t>Declare this local variable with "var"</t>
+  </si>
+  <si>
+    <t>Use StringBuilder instead.</t>
+  </si>
+  <si>
+    <t>File file = new File(filename);</t>
+  </si>
+  <si>
+    <t>It's good practice to have specific variable types.</t>
+  </si>
+  <si>
+    <t>Part.java/line 16</t>
+  </si>
+  <si>
+    <t>Change the visibility of this constructor to protected</t>
+  </si>
+  <si>
+    <t>protected Part(…)</t>
+  </si>
+  <si>
+    <t>public Part(...)</t>
+  </si>
+  <si>
+    <t>Product.java/line 61</t>
+  </si>
+  <si>
+    <t>Remove this useless assignment to local variable "associatedParts"</t>
+  </si>
+  <si>
+    <t>associatedParts = associatedParts</t>
+  </si>
+  <si>
+    <t>this.associatedParts = associatedParts;</t>
+  </si>
+  <si>
+    <t>Product.java/line 99</t>
+  </si>
+  <si>
+    <t>Use "integer.toString" instead</t>
+  </si>
+  <si>
+    <t>new Integer(p.getPartId()).toString().equals(searchItem))</t>
+  </si>
+  <si>
+    <t>p.getPartId().toString().equals(searchItem))</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>Repository class can be a Singleton</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>25 minutes</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 25 minutes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +401,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -420,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -451,7 +541,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -494,6 +583,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,7 +895,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,19 +915,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>27</v>
@@ -850,7 +941,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
@@ -860,15 +951,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="17">
         <v>233</v>
@@ -878,15 +969,15 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="28"/>
+      <c r="D5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="17">
         <v>233</v>
@@ -897,15 +988,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -926,13 +1017,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -941,13 +1032,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -956,13 +1047,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -971,11 +1062,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1091,7 +1182,7 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1115,8 +1206,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,19 +1226,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>27</v>
@@ -1161,7 +1252,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
@@ -1171,15 +1262,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="17">
         <v>233</v>
@@ -1189,15 +1280,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="31"/>
+      <c r="D5" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="17">
         <v>233</v>
@@ -1208,15 +1299,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1237,11 +1328,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1250,24 +1341,24 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1402,7 +1493,7 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1426,8 +1517,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,19 +1538,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>27</v>
@@ -1473,7 +1564,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
@@ -1483,15 +1574,15 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
@@ -1501,15 +1592,15 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="34"/>
+      <c r="D5" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
@@ -1520,15 +1611,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1549,13 +1640,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1564,13 +1655,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1579,13 +1670,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1594,13 +1685,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1761,8 +1852,8 @@
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="22" t="s">
-        <v>42</v>
+      <c r="E32" s="37" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1786,19 +1877,20 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="3" max="3" width="34.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="50" style="6" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
@@ -1808,19 +1900,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>27</v>
@@ -1833,43 +1925,57 @@
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="17">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="17">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="17">
+        <v>233</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1886,54 +1992,94 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -2096,11 +2242,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="C32" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>
@@ -2112,6 +2258,7 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>